<commit_message>
Textos e base entrega 2
</commit_message>
<xml_diff>
--- a/DOCS/Cronograma_Turma_201825166.000.03A_Grupo_Projeto_19.xlsx
+++ b/DOCS/Cronograma_Turma_201825166.000.03A_Grupo_Projeto_19.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ricardo\Documents\ESTUDO\Mackenzie\03_Sem\PROJ_AP_II\PROJETO\Projeto-Aplicado2-Grupo19\DOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ricardo\Documents\ESTUDO\Mackenzie\03_Sem\PROJ_AP_II\PROJETO\Duarte_2025_10_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2C0034-9212-41A9-AE07-41D1CEEE9494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFB9B3F-9E7B-4915-ADF9-F258B4BF79EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15420" yWindow="4730" windowWidth="28240" windowHeight="22220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27480" yWindow="7630" windowWidth="23180" windowHeight="20150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controlador de projetos" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="ColumnTitle1">'Controlador de projetos'!$B$4</definedName>
     <definedName name="ColumnTitle2">Tabela_de_categorias_e_funcionários[[#Headers],[Nome da Categoria]]</definedName>
     <definedName name="Funcionário_Lista">Configuração!$D$5:$D$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Controlador de projetos'!$A$1:$K$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Controlador de projetos'!$A$1:$K$25</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Controlador de projetos'!$4:$4</definedName>
     <definedName name="Sinalizador_Porcentagem">'Controlador de projetos'!#REF!</definedName>
   </definedNames>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="52">
   <si>
     <t>Categoria</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Atualizado em 2025-09-05</t>
+  </si>
+  <si>
+    <t>Documento Fase 2</t>
   </si>
 </sst>
 </file>
@@ -823,7 +826,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -889,12 +892,6 @@
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="13" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="13" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="5" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1200,8 +1197,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ControladorDeProjetos" displayName="ControladorDeProjetos" ref="B4:L32" totalsRowShown="0" tableBorderDxfId="2">
-  <autoFilter ref="B4:L32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ControladorDeProjetos" displayName="ControladorDeProjetos" ref="B4:L33" totalsRowShown="0" tableBorderDxfId="2">
+  <autoFilter ref="B4:L33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarefa" dataCellStyle="Texto"/>
     <tableColumn id="3" xr3:uid="{B833AB72-8646-4CE5-98B8-9D4D27103F03}" name="Responsável" dataCellStyle="Texto"/>
@@ -1476,11 +1473,11 @@
     <tabColor theme="9"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
@@ -1723,46 +1720,46 @@
       <c r="L9" s="12"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1" thickBot="1">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="23">
         <v>45901</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="23">
         <v>45905</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="24">
         <f>IF(COUNTA('Controlador de projetos'!$F10,'Controlador de projetos'!$G10)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F10,'Controlador de projetos'!$G10,FALSE)+1)</f>
         <v>5</v>
       </c>
-      <c r="I10" s="27">
+      <c r="I10" s="25">
         <v>45902</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="23">
         <v>45902</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10" s="26">
         <f>IF(COUNTA('Controlador de projetos'!$I10,'Controlador de projetos'!$J10)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I10,'Controlador de projetos'!$J10,FALSE)+1)</f>
         <v>1</v>
       </c>
-      <c r="L10" s="24"/>
+      <c r="L10" s="22"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="B11" s="12" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>17</v>
@@ -1780,23 +1777,31 @@
         <f>IF(COUNTA('Controlador de projetos'!$F11,'Controlador de projetos'!$G11)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F11,'Controlador de projetos'!$G11,FALSE))</f>
         <v>7</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="15" t="str">
+      <c r="I11" s="13">
+        <v>45913</v>
+      </c>
+      <c r="J11" s="13">
+        <v>45914</v>
+      </c>
+      <c r="K11" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I11,'Controlador de projetos'!$J11)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I11,'Controlador de projetos'!$J11,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L11" s="23"/>
+        <v>1</v>
+      </c>
+      <c r="L11" s="12"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="B12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="12"/>
+      <c r="E12" s="12" t="s">
+        <v>12</v>
+      </c>
       <c r="F12" s="13">
         <v>45908</v>
       </c>
@@ -1804,8 +1809,8 @@
         <v>45933</v>
       </c>
       <c r="H12" s="19">
-        <f>IF(COUNTA('Controlador de projetos'!$F12,'Controlador de projetos'!$G12)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F12,'Controlador de projetos'!$G12,FALSE)+1)</f>
-        <v>26</v>
+        <f>IF(COUNTA('Controlador de projetos'!$F12,'Controlador de projetos'!$G12)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F12,'Controlador de projetos'!$G12,FALSE))</f>
+        <v>25</v>
       </c>
       <c r="I12" s="14">
         <v>45902</v>
@@ -1823,11 +1828,15 @@
       <c r="B13" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="D13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="12"/>
+      <c r="E13" s="12" t="s">
+        <v>12</v>
+      </c>
       <c r="F13" s="13">
         <v>45908</v>
       </c>
@@ -1835,14 +1844,18 @@
         <v>45933</v>
       </c>
       <c r="H13" s="19">
-        <f>IF(COUNTA('Controlador de projetos'!$F13,'Controlador de projetos'!$G13)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F13,'Controlador de projetos'!$G13,FALSE)+1)</f>
-        <v>26</v>
-      </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="15" t="str">
+        <f>IF(COUNTA('Controlador de projetos'!$F13,'Controlador de projetos'!$G13)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F13,'Controlador de projetos'!$G13,FALSE))</f>
+        <v>25</v>
+      </c>
+      <c r="I13" s="14">
+        <v>45928</v>
+      </c>
+      <c r="J13" s="13">
+        <v>45931</v>
+      </c>
+      <c r="K13" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I13,'Controlador de projetos'!$J13)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I13,'Controlador de projetos'!$J13,FALSE)+1)</f>
-        <v/>
+        <v>4</v>
       </c>
       <c r="L13" s="12"/>
     </row>
@@ -1850,11 +1863,15 @@
       <c r="B14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="12"/>
+      <c r="E14" s="12" t="s">
+        <v>12</v>
+      </c>
       <c r="F14" s="13">
         <v>45908</v>
       </c>
@@ -1862,14 +1879,18 @@
         <v>45933</v>
       </c>
       <c r="H14" s="19">
-        <f>IF(COUNTA('Controlador de projetos'!$F14,'Controlador de projetos'!$G14)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F14,'Controlador de projetos'!$G14,FALSE)+1)</f>
-        <v>26</v>
-      </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="15" t="str">
-        <f>IF(COUNTA('Controlador de projetos'!$I14,'Controlador de projetos'!$J14)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I14,'Controlador de projetos'!$J14,FALSE)+1)</f>
-        <v/>
+        <f>IF(COUNTA('Controlador de projetos'!$F14,'Controlador de projetos'!$G14)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F14,'Controlador de projetos'!$G14,FALSE))</f>
+        <v>25</v>
+      </c>
+      <c r="I14" s="14">
+        <v>45928</v>
+      </c>
+      <c r="J14" s="13">
+        <v>45931</v>
+      </c>
+      <c r="K14" s="15">
+        <f>IF(COUNTA('Controlador de projetos'!$I14,'Controlador de projetos'!$J14)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I14,'Controlador de projetos'!$J14,FALSE))</f>
+        <v>3</v>
       </c>
       <c r="L14" s="12"/>
     </row>
@@ -1877,11 +1898,15 @@
       <c r="B15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="12"/>
+      <c r="E15" s="12" t="s">
+        <v>12</v>
+      </c>
       <c r="F15" s="13">
         <v>45908</v>
       </c>
@@ -1892,106 +1917,129 @@
         <f>IF(COUNTA('Controlador de projetos'!$F15,'Controlador de projetos'!$G15)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F15,'Controlador de projetos'!$G15,FALSE))</f>
         <v>25</v>
       </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="15" t="str">
+      <c r="I15" s="14">
+        <v>45931</v>
+      </c>
+      <c r="J15" s="13">
+        <v>45932</v>
+      </c>
+      <c r="K15" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I15,'Controlador de projetos'!$J15)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I15,'Controlador de projetos'!$J15,FALSE))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" ht="30" customHeight="1" thickBot="1">
-      <c r="B16" s="24" t="s">
+    <row r="16" spans="1:12" ht="30" customHeight="1">
+      <c r="B16" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="13">
+        <v>45901</v>
+      </c>
+      <c r="G16" s="13">
+        <v>45933</v>
+      </c>
+      <c r="H16" s="19">
+        <v>33</v>
+      </c>
+      <c r="I16" s="14">
+        <v>45930</v>
+      </c>
+      <c r="J16" s="13">
+        <v>45933</v>
+      </c>
+      <c r="K16" s="15">
+        <f>IF(COUNTA('Controlador de projetos'!$I16,'Controlador de projetos'!$J16)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I16,'Controlador de projetos'!$J16,FALSE))</f>
+        <v>3</v>
+      </c>
+      <c r="L16" s="12"/>
+    </row>
+    <row r="17" spans="2:12" ht="30" customHeight="1" thickBot="1">
+      <c r="B17" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24" t="s">
+      <c r="C17" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="25">
+      <c r="E17" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="23">
         <v>45908</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G17" s="23">
         <v>45933</v>
       </c>
-      <c r="H16" s="26">
-        <f>IF(COUNTA('Controlador de projetos'!$F16,'Controlador de projetos'!$G16)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F16,'Controlador de projetos'!$G16,FALSE))</f>
+      <c r="H17" s="24">
+        <f>IF(COUNTA('Controlador de projetos'!$F17,'Controlador de projetos'!$G17)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F17,'Controlador de projetos'!$G17,FALSE))</f>
         <v>25</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="28" t="str">
-        <f>IF(COUNTA('Controlador de projetos'!$I16,'Controlador de projetos'!$J16)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I16,'Controlador de projetos'!$J16,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L16" s="24"/>
-    </row>
-    <row r="17" spans="2:12" ht="30" customHeight="1">
-      <c r="B17" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="13">
-        <v>45940</v>
-      </c>
-      <c r="G17" s="13">
-        <v>45947</v>
-      </c>
-      <c r="H17" s="19">
-        <v>7</v>
-      </c>
-      <c r="I17" s="22"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="L17" s="23"/>
+      <c r="I17" s="27">
+        <v>45931</v>
+      </c>
+      <c r="J17" s="23">
+        <v>45932</v>
+      </c>
+      <c r="K17" s="26">
+        <f>IF(COUNTA('Controlador de projetos'!$I17,'Controlador de projetos'!$J17)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I17,'Controlador de projetos'!$J17,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="L17" s="22"/>
     </row>
     <row r="18" spans="2:12" ht="30" customHeight="1">
       <c r="B18" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="12"/>
+        <v>48</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="12"/>
+      <c r="E18" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="F18" s="13">
-        <v>45936</v>
+        <v>45940</v>
       </c>
       <c r="G18" s="13">
-        <v>45954</v>
+        <v>45947</v>
       </c>
       <c r="H18" s="19">
-        <f>IF(COUNTA('Controlador de projetos'!$F18,'Controlador de projetos'!$G18)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F18,'Controlador de projetos'!$G18,FALSE)+1)</f>
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="I18" s="14"/>
       <c r="J18" s="13"/>
-      <c r="K18" s="15" t="str">
-        <f>IF(COUNTA('Controlador de projetos'!$I18,'Controlador de projetos'!$J18)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I18,'Controlador de projetos'!$J18,FALSE)+1)</f>
-        <v/>
+      <c r="K18" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="L18" s="12"/>
     </row>
     <row r="19" spans="2:12" ht="30" customHeight="1">
       <c r="B19" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="12"/>
+        <v>39</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="12"/>
+      <c r="E19" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="F19" s="13">
         <v>45936</v>
       </c>
@@ -1999,26 +2047,30 @@
         <v>45954</v>
       </c>
       <c r="H19" s="19">
-        <f>IF(COUNTA('Controlador de projetos'!$F19,'Controlador de projetos'!$G19)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F19,'Controlador de projetos'!$G19,FALSE))</f>
-        <v>18</v>
+        <f>IF(COUNTA('Controlador de projetos'!$F19,'Controlador de projetos'!$G19)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F19,'Controlador de projetos'!$G19,FALSE)+1)</f>
+        <v>19</v>
       </c>
       <c r="I19" s="14"/>
       <c r="J19" s="13"/>
       <c r="K19" s="15" t="str">
-        <f>IF(COUNTA('Controlador de projetos'!$I19,'Controlador de projetos'!$J19)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I19,'Controlador de projetos'!$J19,FALSE))</f>
+        <f>IF(COUNTA('Controlador de projetos'!$I19,'Controlador de projetos'!$J19)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I19,'Controlador de projetos'!$J19,FALSE)+1)</f>
         <v/>
       </c>
       <c r="L19" s="12"/>
     </row>
     <row r="20" spans="2:12" ht="30" customHeight="1">
       <c r="B20" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="12"/>
+        <v>40</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D20" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="12"/>
+      <c r="E20" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="F20" s="13">
         <v>45936</v>
       </c>
@@ -2026,103 +2078,105 @@
         <v>45954</v>
       </c>
       <c r="H20" s="19">
-        <f>IF(COUNTA('Controlador de projetos'!$F20,'Controlador de projetos'!$G20)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F20,'Controlador de projetos'!$G20,FALSE)+1)</f>
-        <v>19</v>
+        <f>IF(COUNTA('Controlador de projetos'!$F20,'Controlador de projetos'!$G20)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F20,'Controlador de projetos'!$G20,FALSE))</f>
+        <v>18</v>
       </c>
       <c r="I20" s="14"/>
       <c r="J20" s="13"/>
       <c r="K20" s="15" t="str">
-        <f>IF(COUNTA('Controlador de projetos'!$I20,'Controlador de projetos'!$J20)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I20,'Controlador de projetos'!$J20,FALSE)+1)</f>
+        <f>IF(COUNTA('Controlador de projetos'!$I20,'Controlador de projetos'!$J20)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I20,'Controlador de projetos'!$J20,FALSE))</f>
         <v/>
       </c>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="2:12" ht="30" customHeight="1" thickBot="1">
-      <c r="B21" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24" t="s">
+    <row r="21" spans="2:12" ht="30" customHeight="1">
+      <c r="B21" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="24"/>
-      <c r="F21" s="25">
+      <c r="E21" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="13">
         <v>45936</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="13">
         <v>45954</v>
       </c>
-      <c r="H21" s="26">
+      <c r="H21" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F21,'Controlador de projetos'!$G21)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F21,'Controlador de projetos'!$G21,FALSE)+1)</f>
         <v>19</v>
       </c>
-      <c r="I21" s="29"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="28" t="str">
+      <c r="I21" s="14"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="15" t="str">
         <f>IF(COUNTA('Controlador de projetos'!$I21,'Controlador de projetos'!$J21)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I21,'Controlador de projetos'!$J21,FALSE)+1)</f>
         <v/>
       </c>
-      <c r="L21" s="24"/>
-    </row>
-    <row r="22" spans="2:12" ht="30" customHeight="1">
-      <c r="B22" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="12" t="s">
+      <c r="L21" s="12"/>
+    </row>
+    <row r="22" spans="2:12" ht="30" customHeight="1" thickBot="1">
+      <c r="B22" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="22"/>
+      <c r="F22" s="23">
+        <v>45936</v>
+      </c>
+      <c r="G22" s="23">
+        <v>45954</v>
+      </c>
+      <c r="H22" s="24">
+        <f>IF(COUNTA('Controlador de projetos'!$F22,'Controlador de projetos'!$G22)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F22,'Controlador de projetos'!$G22,FALSE)+1)</f>
         <v>19</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="13">
-        <v>45962</v>
-      </c>
-      <c r="G22" s="13">
-        <v>45969</v>
-      </c>
-      <c r="H22" s="19">
-        <v>7</v>
-      </c>
-      <c r="I22" s="22"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="L22" s="23"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="26" t="str">
+        <f>IF(COUNTA('Controlador de projetos'!$I22,'Controlador de projetos'!$J22)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I22,'Controlador de projetos'!$J22,FALSE)+1)</f>
+        <v/>
+      </c>
+      <c r="L22" s="22"/>
     </row>
     <row r="23" spans="2:12" ht="30" customHeight="1">
       <c r="B23" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="12"/>
+        <v>49</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D23" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="12"/>
+      <c r="E23" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="F23" s="13">
-        <v>45957</v>
+        <v>45962</v>
       </c>
       <c r="G23" s="13">
-        <v>45982</v>
+        <v>45969</v>
       </c>
       <c r="H23" s="19">
-        <f>IF(COUNTA('Controlador de projetos'!$F23,'Controlador de projetos'!$G23)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F23,'Controlador de projetos'!$G23,FALSE)+1)</f>
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="I23" s="14"/>
       <c r="J23" s="13"/>
-      <c r="K23" s="15" t="str">
-        <f>IF(COUNTA('Controlador de projetos'!$I23,'Controlador de projetos'!$J23)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I23,'Controlador de projetos'!$J23,FALSE)+1)</f>
-        <v/>
+      <c r="K23" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="L23" s="12"/>
     </row>
     <row r="24" spans="2:12" ht="30" customHeight="1">
       <c r="B24" s="12" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="12" t="s">
@@ -2149,7 +2203,7 @@
     </row>
     <row r="25" spans="2:12" ht="30" customHeight="1">
       <c r="B25" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="12" t="s">
@@ -2174,51 +2228,59 @@
       </c>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="2:12" ht="30" customHeight="1" thickBot="1">
-      <c r="B26" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24" t="s">
+    <row r="26" spans="2:12" ht="30" customHeight="1">
+      <c r="B26" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="24"/>
-      <c r="F26" s="25">
+      <c r="E26" s="12"/>
+      <c r="F26" s="13">
         <v>45957</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="13">
         <v>45982</v>
       </c>
-      <c r="H26" s="26">
+      <c r="H26" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F26,'Controlador de projetos'!$G26)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F26,'Controlador de projetos'!$G26,FALSE)+1)</f>
         <v>25</v>
       </c>
-      <c r="I26" s="29"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="28" t="str">
+      <c r="I26" s="14"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="15" t="str">
         <f>IF(COUNTA('Controlador de projetos'!$I26,'Controlador de projetos'!$J26)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I26,'Controlador de projetos'!$J26,FALSE)+1)</f>
         <v/>
       </c>
-      <c r="L26" s="24"/>
-    </row>
-    <row r="27" spans="2:12" ht="30" customHeight="1">
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="19" t="str">
+      <c r="L26" s="12"/>
+    </row>
+    <row r="27" spans="2:12" ht="30" customHeight="1" thickBot="1">
+      <c r="B27" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="22"/>
+      <c r="F27" s="23">
+        <v>45957</v>
+      </c>
+      <c r="G27" s="23">
+        <v>45982</v>
+      </c>
+      <c r="H27" s="24">
         <f>IF(COUNTA('Controlador de projetos'!$F27,'Controlador de projetos'!$G27)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F27,'Controlador de projetos'!$G27,FALSE)+1)</f>
-        <v/>
-      </c>
-      <c r="I27" s="14"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="15" t="str">
+        <v>25</v>
+      </c>
+      <c r="I27" s="27"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="26" t="str">
         <f>IF(COUNTA('Controlador de projetos'!$I27,'Controlador de projetos'!$J27)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I27,'Controlador de projetos'!$J27,FALSE)+1)</f>
         <v/>
       </c>
-      <c r="L27" s="12"/>
+      <c r="L27" s="22"/>
     </row>
     <row r="28" spans="2:12" ht="30" customHeight="1">
       <c r="B28" s="12"/>
@@ -2297,26 +2359,45 @@
       <c r="L31" s="12"/>
     </row>
     <row r="32" spans="2:12" ht="30" customHeight="1">
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
       <c r="H32" s="19" t="str">
         <f>IF(COUNTA('Controlador de projetos'!$F32,'Controlador de projetos'!$G32)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F32,'Controlador de projetos'!$G32,FALSE)+1)</f>
         <v/>
       </c>
       <c r="I32" s="14"/>
-      <c r="J32" s="17"/>
+      <c r="J32" s="13"/>
       <c r="K32" s="15" t="str">
         <f>IF(COUNTA('Controlador de projetos'!$I32,'Controlador de projetos'!$J32)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I32,'Controlador de projetos'!$J32,FALSE)+1)</f>
         <v/>
       </c>
-      <c r="L32" s="16"/>
+      <c r="L32" s="12"/>
+    </row>
+    <row r="33" spans="2:12" ht="30" customHeight="1">
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="19" t="str">
+        <f>IF(COUNTA('Controlador de projetos'!$F33,'Controlador de projetos'!$G33)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F33,'Controlador de projetos'!$G33,FALSE)+1)</f>
+        <v/>
+      </c>
+      <c r="I33" s="14"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="15" t="str">
+        <f>IF(COUNTA('Controlador de projetos'!$I33,'Controlador de projetos'!$J33)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I33,'Controlador de projetos'!$J33,FALSE)+1)</f>
+        <v/>
+      </c>
+      <c r="L33" s="16"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K5:K32">
+  <conditionalFormatting sqref="K5:K33">
     <cfRule type="expression" dxfId="0" priority="8">
       <formula>(ABS((K5-H5))/H5)&gt;Sinalizador_Porcentagem</formula>
     </cfRule>
@@ -2332,7 +2413,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a data de término real do projeto nesta coluna" sqref="J4" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a duração real de projeto em dias. Valores que atendem aos critérios Acima/Abaixo são destacados em negrito vermelho e geram um ícone de sinalizador na coluna M à esquerda" sqref="K4" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira anotações para os projetos nesta coluna" sqref="L4" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione uma categoria na lista ou crie uma nova categoria para exibir nesta lista da planilha Configuração." sqref="E5:E32" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione uma categoria na lista ou crie uma nova categoria para exibir nesta lista da planilha Configuração." sqref="E5:E33" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Categoria_Lista</formula1>
     </dataValidation>
   </dataValidations>
@@ -2353,13 +2434,13 @@
           <x14:formula1>
             <xm:f>Configuração!$D$5:$D$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D32</xm:sqref>
+          <xm:sqref>D5:D33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9316C738-7C0B-41CA-ADB5-1A14C6ABE9FF}">
           <x14:formula1>
             <xm:f>Configuração!$C$5:$C$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C32</xm:sqref>
+          <xm:sqref>C5:C33</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>